<commit_message>
new (also if commented) vertical modifier among tree height classes (instead layers) new files for ISIMIP
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/tables/vertical_light_modifier.xlsx
+++ b/software/3D-CMCC-Forest-Model/tables/vertical_light_modifier.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>H dominant</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>normalized dominated</t>
+  </si>
+  <si>
+    <t>H/d</t>
   </si>
 </sst>
 </file>
@@ -78,6 +81,343 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.92974708404197082</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8745041071331906</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81427612575505981</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75605120600834608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70227999014135933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65342870042331347</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60924600792511929</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56926713483559743</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53300202447578893</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="61126912"/>
+        <c:axId val="63011456"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="61126912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="63011456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="63011456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61126912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dominant modifier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.96922131470585315</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92974708404197082</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8745041071331906</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81427612575505981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75605120600834608</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70227999014135933</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65342870042331347</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60924600792511929</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56926713483559743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.53300202447578893</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dominated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.0778685294146846E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0252915958029183E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1254958928668094</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18572387424494019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24394879399165392</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29772000985864067</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34657129957668653</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39075399207488071</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43073286516440257</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.46699797552421107</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="71390336"/>
+        <c:axId val="71391872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="71390336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71391872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71391872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71390336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,20 +705,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D1" sqref="D1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,197 +727,245 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="e">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>A2/B2</f>
+        <v>11</v>
+      </c>
+      <c r="D2">
         <f>0.5*(1+(2^(-B2/A2))-(2^(-A2/B2)))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" t="e">
-        <f>1-C2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0.96922131470585315</v>
+      </c>
+      <c r="E2">
+        <f>1-D2</f>
+        <v>3.0778685294146846E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C12" si="0">A3/B3</f>
+        <v>5.5</v>
+      </c>
+      <c r="D3">
         <f>0.5*(1+(2^(-B3/A3))-(2^(-A3/B3)))</f>
-        <v>0.96602821451840371</v>
-      </c>
-      <c r="D3">
-        <f>1-C3</f>
-        <v>3.3971785481596295E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>0.92974708404197082</v>
+      </c>
+      <c r="E3">
+        <f>1-D3</f>
+        <v>7.0252915958029183E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C12" si="0">0.5*(1+(2^(-B4/A4))-(2^(-A4/B4)))</f>
-        <v>0.91965028164806206</v>
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" si="1">1-C4</f>
-        <v>8.0349718351937938E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f t="shared" ref="D4:D12" si="1">0.5*(1+(2^(-B4/A4))-(2^(-A4/B4)))</f>
+        <v>0.8745041071331906</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="2">1-D4</f>
+        <v>0.1254958928668094</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.85651991530411142</v>
+        <v>2.75</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>0.14348008469588858</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0.81427612575505981</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.18572387424494019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.79054079397928101</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>0.20945920602071899</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>0.75605120600834608</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.24394879399165392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.72855339059327373</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>0.27144660940672627</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>0.70227999014135933</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.29772000985864067</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.67238684645636437</v>
+        <v>1.5714285714285714</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>0.32761315354363563</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>0.65342870042331347</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.34657129957668653</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.62203681719411041</v>
+        <v>1.375</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>0.37796318280588959</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>0.60924600792511929</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.39075399207488071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.57695048493583001</v>
+        <v>1.2222222222222223</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>0.42304951506416999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>0.56926713483559743</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.43073286516440257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
         <v>10</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.5364746875622507</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>0.4635253124377493</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>0.53300202447578893</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0.46699797552421107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
attempts to fix bugs when two layers merges
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/tables/vertical_light_modifier.xlsx
+++ b/software/3D-CMCC-Forest-Model/tables/vertical_light_modifier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="10110" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="vertical" sheetId="1" r:id="rId1"/>
+    <sheet name="verical  horizontal" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>H dominant</t>
   </si>
   <si>
     <t>h dominated</t>
-  </si>
-  <si>
-    <t>dominant modifier</t>
-  </si>
-  <si>
-    <t>dominated</t>
   </si>
   <si>
     <t>normalized dominant</t>
@@ -38,11 +32,29 @@
   <si>
     <t>H/d</t>
   </si>
+  <si>
+    <t>dominant vertical  modifier</t>
+  </si>
+  <si>
+    <t>dominated vertical  modifier</t>
+  </si>
+  <si>
+    <t>canopy coverage proj</t>
+  </si>
+  <si>
+    <t>vertical (0.969222) + horizontal</t>
+  </si>
+  <si>
+    <t>vertical (0.5) + horizontal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -52,15 +64,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -68,12 +92,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -99,9 +167,9 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$3:$D$12</c:f>
+              <c:f>vertical!$D$3:$D$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.92974708404197082</c:v>
@@ -138,32 +206,32 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="61126912"/>
-        <c:axId val="63011456"/>
+        <c:axId val="89884160"/>
+        <c:axId val="89885696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61126912"/>
+        <c:axId val="89884160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63011456"/>
+        <c:crossAx val="89885696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63011456"/>
+        <c:axId val="89885696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61126912"/>
+        <c:crossAx val="89884160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -176,7 +244,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -195,11 +263,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$D$1</c:f>
+              <c:f>vertical!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>dominant modifier</c:v>
+                  <c:v>dominant vertical  modifier</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -209,9 +277,9 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$2:$D$12</c:f>
+              <c:f>vertical!$D$2:$D$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.96922131470585315</c:v>
@@ -255,11 +323,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$E$1</c:f>
+              <c:f>vertical!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>dominated</c:v>
+                  <c:v>dominated vertical  modifier</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -269,9 +337,9 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$E$2:$E$12</c:f>
+              <c:f>vertical!$E$2:$E$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>3.0778685294146846E-2</c:v>
@@ -311,24 +379,191 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71390336"/>
-        <c:axId val="71391872"/>
+        <c:axId val="91896832"/>
+        <c:axId val="91910912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71390336"/>
+        <c:axId val="91896832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71391872"/>
+        <c:crossAx val="91910912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71391872"/>
+        <c:axId val="91910912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91896832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'verical  horizontal'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vertical (0.969222) + horizontal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'verical  horizontal'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.6922131470585315E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19384426294117063</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29076639441175595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38768852588234126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48461065735292658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58153278882351189</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67845492029409715</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77537705176468252</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87229918323526789</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96922131470585315</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'verical  horizontal'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vertical (0.5) + horizontal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'verical  horizontal'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="54545408"/>
+        <c:axId val="54551296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="54545408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54551296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54551296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,7 +571,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71390336"/>
+        <c:crossAx val="54545408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -412,6 +647,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -707,16 +977,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -726,20 +997,20 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -749,15 +1020,15 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>A2/B2</f>
         <v>11</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>0.5*(1+(2^(-B2/A2))-(2^(-A2/B2)))</f>
         <v>0.96922131470585315</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>1-D2</f>
         <v>3.0778685294146846E-2</v>
       </c>
@@ -769,15 +1040,15 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C12" si="0">A3/B3</f>
         <v>5.5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>0.5*(1+(2^(-B3/A3))-(2^(-A3/B3)))</f>
         <v>0.92974708404197082</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f>1-D3</f>
         <v>7.0252915958029183E-2</v>
       </c>
@@ -789,15 +1060,15 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" ref="D4:D12" si="1">0.5*(1+(2^(-B4/A4))-(2^(-A4/B4)))</f>
         <v>0.8745041071331906</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f t="shared" ref="E4:E12" si="2">1-D4</f>
         <v>0.1254958928668094</v>
       </c>
@@ -809,15 +1080,15 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>0.81427612575505981</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
         <v>0.18572387424494019</v>
       </c>
@@ -829,15 +1100,15 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>0.75605120600834608</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
         <v>0.24394879399165392</v>
       </c>
@@ -849,15 +1120,15 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>0.70227999014135933</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>0.29772000985864067</v>
       </c>
@@ -869,15 +1140,15 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>1.5714285714285714</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>0.65342870042331347</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>0.34657129957668653</v>
       </c>
@@ -889,15 +1160,15 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>1.375</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>0.60924600792511929</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
         <v>0.39075399207488071</v>
       </c>
@@ -909,15 +1180,15 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>1.2222222222222223</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>0.56926713483559743</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
         <v>0.43073286516440257</v>
       </c>
@@ -929,15 +1200,15 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>0.53300202447578893</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
         <v>0.46699797552421107</v>
       </c>
@@ -949,36 +1220,224 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6">
+        <v>0.96922131470585315</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <f>$A$2*B2</f>
+        <v>9.6922131470585315E-2</v>
+      </c>
+      <c r="D2">
+        <f>$A$12*B2</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6">
+        <v>0.92974708404197082</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C11" si="0">$A$2*B3</f>
+        <v>0.19384426294117063</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="1">$A$12*B3</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="6">
+        <v>0.8745041071331906</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.29076639441175595</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="6">
+        <v>0.81427612575505981</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.38768852588234126</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6">
+        <v>0.75605120600834608</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.48461065735292658</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6">
+        <v>0.70227999014135933</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.58153278882351189</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6">
+        <v>0.65342870042331347</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.67845492029409715</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6">
+        <v>0.60924600792511929</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.77537705176468252</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6">
+        <v>0.56926713483559743</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.87229918323526789</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="6">
+        <v>0.53300202447578893</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.96922131470585315</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>